<commit_message>
Chỉnh sửa phần giao diện file ui
</commit_message>
<xml_diff>
--- a/docs/name_variable_in_gui.xlsx
+++ b/docs/name_variable_in_gui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRONICS DOC\Project_CV_tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_with_Data_Pronics\Computer_Vision_Tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1DFBE1-CDBE-46B7-8AF5-5FB7720254CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC04719A-6603-4F5B-A4B3-060A44E0E394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="19416" xr2:uid="{8C762027-7354-427E-B1FD-32CB6FB492B5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{8C762027-7354-427E-B1FD-32CB6FB492B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -135,45 +126,18 @@
     <t>Combobox2</t>
   </si>
   <si>
-    <t>btn_cbb1</t>
-  </si>
-  <si>
-    <t>btn_cbb2</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
     <t>List widget</t>
   </si>
   <si>
-    <t>lw_1</t>
-  </si>
-  <si>
     <t>EXIT</t>
   </si>
   <si>
     <t>btn_exit</t>
   </si>
   <si>
-    <t>lb_1</t>
-  </si>
-  <si>
-    <t>lb_2</t>
-  </si>
-  <si>
-    <t>lb_3</t>
-  </si>
-  <si>
-    <t>fd_1</t>
-  </si>
-  <si>
-    <t>fd_2</t>
-  </si>
-  <si>
-    <t>fd_3</t>
-  </si>
-  <si>
     <t>btn_polyundo</t>
   </si>
   <si>
@@ -183,40 +147,46 @@
     <t>btn_realtime</t>
   </si>
   <si>
-    <t>stackWidget</t>
-  </si>
-  <si>
-    <t>sw_1</t>
-  </si>
-  <si>
-    <t>page1inSW</t>
-  </si>
-  <si>
-    <t>page2inSW</t>
-  </si>
-  <si>
-    <t>lb_4</t>
-  </si>
-  <si>
-    <t>lb_5</t>
-  </si>
-  <si>
     <t>LabelCheck1</t>
   </si>
   <si>
-    <t>LabelCheck2</t>
-  </si>
-  <si>
-    <t>LabelCheck3</t>
-  </si>
-  <si>
-    <t>FindCheck1</t>
-  </si>
-  <si>
-    <t>FindCheck2</t>
-  </si>
-  <si>
-    <t>FindCheck3</t>
+    <t>btn_shape</t>
+  </si>
+  <si>
+    <t>btn_color</t>
+  </si>
+  <si>
+    <t>list_image</t>
+  </si>
+  <si>
+    <t>label show main</t>
+  </si>
+  <si>
+    <t>label show subwindow</t>
+  </si>
+  <si>
+    <t>screen_subwindow_1</t>
+  </si>
+  <si>
+    <t>screen_main</t>
+  </si>
+  <si>
+    <t>Button Sample</t>
+  </si>
+  <si>
+    <t>btn_sample_1-11</t>
+  </si>
+  <si>
+    <t>label_sample_1-11</t>
+  </si>
+  <si>
+    <t>stackWidget --&gt; stackwidget</t>
+  </si>
+  <si>
+    <t>page_main</t>
+  </si>
+  <si>
+    <t>page_sub_1</t>
   </si>
 </sst>
 </file>
@@ -245,15 +215,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -276,14 +258,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,23 +593,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9C5EF2-1490-41F8-A5F4-D149A0323EAC}">
-  <dimension ref="C4:E33"/>
+  <dimension ref="B4:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="3" width="8.90625" style="1"/>
+    <col min="4" max="4" width="30.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -622,8 +618,9 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -633,8 +630,9 @@
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C6" s="2">
         <v>2</v>
       </c>
@@ -644,8 +642,9 @@
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C7" s="2">
         <v>3</v>
       </c>
@@ -655,8 +654,9 @@
       <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C8" s="2">
         <v>4</v>
       </c>
@@ -666,284 +666,335 @@
       <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.45">
       <c r="C9" s="2">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C11" s="2">
         <v>6</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C12" s="2">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C10" s="2">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C11" s="2">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C14" s="2">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C12" s="2">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C15" s="2">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C13" s="2">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.45">
+      <c r="C16" s="2">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C18" s="2">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C19" s="2">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C20" s="2">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C21" s="2">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C22" s="2">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C23" s="2">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C24" s="2">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C25" s="2">
+        <v>18</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C26" s="2">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C14" s="2">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C15" s="2">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C16" s="2">
-        <v>12</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="2" t="s">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C27" s="2">
+        <v>20</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C28" s="2">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C29" s="2">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C30" s="2">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C17" s="2">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="2">
-        <v>14</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="2">
-        <v>15</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C20" s="2">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C21" s="2">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="2">
-        <v>18</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C23" s="2">
-        <v>19</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="2">
-        <v>20</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C25" s="2">
-        <v>21</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C26" s="2">
-        <v>22</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C27" s="2">
-        <v>23</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C28" s="2">
-        <v>24</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C29" s="2">
-        <v>25</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C30" s="2">
-        <v>26</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C31" s="2">
-        <v>27</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C32" s="2">
-        <v>28</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="2" t="s">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C33" s="2">
-        <v>29</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="F31" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhập bản tạm thời của Mouse Tool- OBB
</commit_message>
<xml_diff>
--- a/docs/name_variable_in_gui.xlsx
+++ b/docs/name_variable_in_gui.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_with_Data_Pronics\Computer_Vision_Tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC04719A-6603-4F5B-A4B3-060A44E0E394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5893E-DBB8-4EB0-AECE-F98A22F8F07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{8C762027-7354-427E-B1FD-32CB6FB492B5}"/>
   </bookViews>
@@ -271,11 +271,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -595,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9C5EF2-1490-41F8-A5F4-D149A0323EAC}">
   <dimension ref="B4:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -758,13 +757,13 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C18" s="2">
         <v>11</v>
       </c>
@@ -776,7 +775,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C19" s="2">
         <v>12</v>
       </c>
@@ -788,7 +787,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C20" s="2">
         <v>13</v>
       </c>
@@ -800,7 +799,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C21" s="2">
         <v>14</v>
       </c>
@@ -812,7 +811,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C22" s="2">
         <v>15</v>
       </c>
@@ -824,7 +823,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C23" s="2">
         <v>16</v>
       </c>
@@ -836,7 +835,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C24" s="2">
         <v>17</v>
       </c>
@@ -848,7 +847,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C25" s="2">
         <v>18</v>
       </c>
@@ -860,7 +859,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C26" s="2">
         <v>19</v>
       </c>
@@ -878,7 +877,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C27" s="2">
         <v>20</v>
       </c>
@@ -890,7 +889,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C28" s="2">
         <v>21</v>
       </c>
@@ -902,7 +901,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C29" s="2">
         <v>22</v>
       </c>
@@ -914,83 +913,36 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C30" s="2">
         <v>23</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Hoàn thiện tool liên quan đến các hình còn lại Circle, Polygon, Oriented Box
</commit_message>
<xml_diff>
--- a/docs/name_variable_in_gui.xlsx
+++ b/docs/name_variable_in_gui.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_with_Data_Pronics\Computer_Vision_Tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5893E-DBB8-4EB0-AECE-F98A22F8F07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66685632-2DA7-4CC6-876D-B709EECEF23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{8C762027-7354-427E-B1FD-32CB6FB492B5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -159,12 +159,6 @@
     <t>list_image</t>
   </si>
   <si>
-    <t>label show main</t>
-  </si>
-  <si>
-    <t>label show subwindow</t>
-  </si>
-  <si>
     <t>screen_subwindow_1</t>
   </si>
   <si>
@@ -187,6 +181,18 @@
   </si>
   <si>
     <t>page_sub_1</t>
+  </si>
+  <si>
+    <t>label_camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE: </t>
+  </si>
+  <si>
+    <t>Combobox3</t>
+  </si>
+  <si>
+    <t>btn_resize</t>
   </si>
 </sst>
 </file>
@@ -594,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9C5EF2-1490-41F8-A5F4-D149A0323EAC}">
   <dimension ref="B4:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -765,7 +771,7 @@
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C18" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>11</v>
@@ -777,7 +783,7 @@
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C19" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
@@ -789,7 +795,7 @@
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C20" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>13</v>
@@ -801,7 +807,7 @@
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C21" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>14</v>
@@ -813,7 +819,7 @@
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C22" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>15</v>
@@ -825,7 +831,7 @@
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C23" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>16</v>
@@ -837,7 +843,7 @@
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C24" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>17</v>
@@ -848,16 +854,10 @@
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C25" s="2">
-        <v>18</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C26" s="2">
@@ -870,12 +870,8 @@
         <v>42</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="J26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C27" s="2">
@@ -897,7 +893,7 @@
         <v>40</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -906,10 +902,10 @@
         <v>22</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -918,24 +914,54 @@
         <v>23</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C33" s="2">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="E33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C34" s="2">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="2"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>

</xml_diff>

<commit_message>
Đã gần hoàn thiện xong phần Sample bên hông và đang trong quá trình chỉ sửa phần còn lại, cái này marge với main cho Ken làm việc
</commit_message>
<xml_diff>
--- a/docs/name_variable_in_gui.xlsx
+++ b/docs/name_variable_in_gui.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_with_Data_Pronics\Computer_Vision_Tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66685632-2DA7-4CC6-876D-B709EECEF23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D091609-222D-4B4F-B475-EBBB54DD381C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{8C762027-7354-427E-B1FD-32CB6FB492B5}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="11710" xr2:uid="{8C762027-7354-427E-B1FD-32CB6FB492B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>btn_realtime</t>
   </si>
   <si>
-    <t>LabelCheck1</t>
-  </si>
-  <si>
     <t>btn_shape</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>btn_sample_1-11</t>
   </si>
   <si>
-    <t>label_sample_1-11</t>
-  </si>
-  <si>
     <t>stackWidget --&gt; stackwidget</t>
   </si>
   <si>
@@ -193,6 +187,42 @@
   </si>
   <si>
     <t>btn_resize</t>
+  </si>
+  <si>
+    <t>Button Stick</t>
+  </si>
+  <si>
+    <t>btn_stick_1-11</t>
+  </si>
+  <si>
+    <t>Button Delete</t>
+  </si>
+  <si>
+    <t>btn_delete_1-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button check camera </t>
+  </si>
+  <si>
+    <t>Button capture</t>
+  </si>
+  <si>
+    <t>Button choose camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label size </t>
+  </si>
+  <si>
+    <t>btn_check_cam</t>
+  </si>
+  <si>
+    <t>btn_choose_cam</t>
+  </si>
+  <si>
+    <t>btn_capture_cam</t>
+  </si>
+  <si>
+    <t>lb_size_cam</t>
   </si>
 </sst>
 </file>
@@ -598,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9C5EF2-1490-41F8-A5F4-D149A0323EAC}">
-  <dimension ref="B4:K39"/>
+  <dimension ref="B4:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -699,7 +729,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -867,7 +897,7 @@
         <v>32</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2"/>
       <c r="J26" s="2"/>
@@ -881,7 +911,7 @@
         <v>34</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -890,10 +920,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -902,73 +932,117 @@
         <v>22</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C30" s="2">
-        <v>23</v>
-      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C32" s="2">
+        <v>23</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C35" s="2">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C33" s="2">
-        <v>24</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C36" s="2">
+        <v>25</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C34" s="2">
-        <v>25</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="D39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>